<commit_message>
Structure and RHS of Mph sub-model were corrected
</commit_message>
<xml_diff>
--- a/data/Cyotocon_cytokines/20200614_05-03-57_IL1b_modified.xlsx
+++ b/data/Cyotocon_cytokines/20200614_05-03-57_IL1b_modified.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\oleg\COVID19\covid19-qsp-model\data\Cyotocon_cytokines\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E3C800F0-E636-4DC7-81C3-C4ED1FD631E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A837092F-C7C7-40E6-AE03-785F6FFDC549}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="20200614_05-03-57_IL1b" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,15 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'20200614_05-03-57_IL1b'!$A$1:$AN$28</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="181029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -307,7 +315,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1168,11 +1176,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AN32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3336,7 +3347,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AN28"/>
+  <autoFilter ref="A1:AN28" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>